<commit_message>
minor doc classes change
</commit_message>
<xml_diff>
--- a/Classes and attributes.xlsx
+++ b/Classes and attributes.xlsx
@@ -777,7 +777,7 @@
   <dimension ref="A1:N56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,13 +843,13 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>26</v>
@@ -858,7 +858,7 @@
       <c r="F3" s="19"/>
       <c r="G3" s="19"/>
       <c r="H3" s="19">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>92</v>
@@ -866,13 +866,13 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>26</v>
@@ -881,81 +881,79 @@
       <c r="F4" s="19"/>
       <c r="G4" s="19"/>
       <c r="H4" s="19">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
-        <v>16</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E5" s="10">
-        <v>10</v>
-      </c>
-      <c r="F5" s="10">
-        <v>0</v>
-      </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10">
-        <v>20</v>
+      <c r="A5" s="14">
+        <v>13</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19">
+        <v>32</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
-        <v>17</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E6" s="10">
-        <v>15</v>
-      </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10">
-        <v>20</v>
+      <c r="A6" s="14">
+        <v>14</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19">
+        <v>10</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14">
-        <v>12</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19">
+      <c r="A7" s="6">
+        <v>15</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" s="10">
+        <v>300</v>
+      </c>
+      <c r="F7" s="10">
+        <v>2</v>
+      </c>
+      <c r="G7" s="10">
+        <v>5</v>
+      </c>
+      <c r="H7" s="10">
         <v>30</v>
       </c>
       <c r="J7" s="5" t="s">
@@ -964,517 +962,507 @@
     </row>
     <row r="8" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
+        <v>16</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E8" s="10">
+        <v>10</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0</v>
+      </c>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>17</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E9" s="10">
         <v>15</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="E8" s="10">
-        <v>300</v>
-      </c>
-      <c r="F8" s="10">
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>18</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E10" s="10">
+        <v>150</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>20.5</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11">
+        <v>1</v>
+      </c>
+      <c r="H12" s="11">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>21</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" s="11">
+        <v>400</v>
+      </c>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>22</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>23</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11">
         <v>2</v>
       </c>
-      <c r="G8" s="10">
-        <v>5</v>
-      </c>
-      <c r="H8" s="10">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>22</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>30</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E10" s="12">
-        <v>500</v>
-      </c>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>31</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="E11" s="12">
-        <v>310</v>
-      </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12">
-        <v>1</v>
-      </c>
-      <c r="H11" s="12">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>32</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12">
-        <v>1</v>
-      </c>
-      <c r="H12" s="12">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14">
-        <v>13</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>33</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12">
-        <v>1</v>
-      </c>
-      <c r="H14" s="12">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>34</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12">
-        <v>4</v>
-      </c>
-      <c r="H15" s="12">
-        <v>35</v>
+      <c r="H15" s="11">
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>36</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12">
-        <v>37</v>
+      <c r="A16" s="2">
+        <v>24</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E16" s="11">
+        <v>350</v>
+      </c>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11">
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
+        <v>30</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E17" s="12">
+        <v>500</v>
+      </c>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>31</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E18" s="12">
+        <v>310</v>
+      </c>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12">
+        <v>1</v>
+      </c>
+      <c r="H18" s="12">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>32</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12">
+        <v>1</v>
+      </c>
+      <c r="H19" s="12">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>33</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12">
+        <v>1</v>
+      </c>
+      <c r="H20" s="12">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>34</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12">
+        <v>4</v>
+      </c>
+      <c r="H21" s="12">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>35</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12">
+        <v>4</v>
+      </c>
+      <c r="H22" s="12">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>36</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>37</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12">
+        <v>3</v>
+      </c>
+      <c r="H24" s="12">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
         <v>38</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B25" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E25" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12" t="s">
+      <c r="F25" s="12"/>
+      <c r="G25" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H25" s="12">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
+    <row r="26" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>39</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26" s="12"/>
+      <c r="G26" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="H26" s="12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>39.5</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H27" s="12">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
         <v>40</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B28" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C28" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D28" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E28" s="13">
         <v>110</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F28" s="13">
         <v>1</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G28" s="13">
         <v>2</v>
       </c>
-      <c r="H18" s="13">
+      <c r="H28" s="13">
         <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
-        <v>42</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E19" s="13">
-        <v>130</v>
-      </c>
-      <c r="F19" s="13">
-        <v>1</v>
-      </c>
-      <c r="G19" s="13">
-        <v>1</v>
-      </c>
-      <c r="H19" s="13">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
-        <v>44</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E20" s="13">
-        <v>100</v>
-      </c>
-      <c r="F20" s="13">
-        <v>1</v>
-      </c>
-      <c r="G20" s="13">
-        <v>1</v>
-      </c>
-      <c r="H20" s="13">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
-        <v>45</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="E21" s="13">
-        <v>20</v>
-      </c>
-      <c r="F21" s="13">
-        <v>4</v>
-      </c>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
-        <v>49</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E22" s="13">
-        <v>290</v>
-      </c>
-      <c r="F22" s="13">
-        <v>3</v>
-      </c>
-      <c r="G22" s="13">
-        <v>1</v>
-      </c>
-      <c r="H22" s="13">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6">
-        <v>18</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="E23" s="10">
-        <v>150</v>
-      </c>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
-        <v>46</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E24" s="13">
-        <v>140</v>
-      </c>
-      <c r="F24" s="13">
-        <v>1</v>
-      </c>
-      <c r="G24" s="13">
-        <v>1</v>
-      </c>
-      <c r="H24" s="13">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>20</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>21</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E26" s="11">
-        <v>400</v>
-      </c>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
-        <v>43</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="E27" s="13">
-        <v>120</v>
-      </c>
-      <c r="F27" s="13">
-        <v>1</v>
-      </c>
-      <c r="G27" s="13">
-        <v>2</v>
-      </c>
-      <c r="H27" s="13">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>20.5</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11">
-        <v>1</v>
-      </c>
-      <c r="H28" s="11">
-        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>91</v>
+        <v>107</v>
       </c>
       <c r="E29" s="13">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="F29" s="13">
         <v>2</v>
@@ -1483,201 +1471,213 @@
         <v>3</v>
       </c>
       <c r="H29" s="13">
-        <v>70</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>91</v>
       </c>
       <c r="E30" s="13">
-        <v>210</v>
+        <v>130</v>
       </c>
       <c r="F30" s="13">
+        <v>1</v>
+      </c>
+      <c r="G30" s="13">
+        <v>1</v>
+      </c>
+      <c r="H30" s="13">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>43</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E31" s="13">
+        <v>120</v>
+      </c>
+      <c r="F31" s="13">
+        <v>1</v>
+      </c>
+      <c r="G31" s="13">
         <v>2</v>
       </c>
-      <c r="G30" s="13">
-        <v>2</v>
-      </c>
-      <c r="H30" s="13">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <v>23</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11">
-        <v>2</v>
-      </c>
-      <c r="H31" s="11">
-        <v>75</v>
+      <c r="H31" s="13">
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <v>24</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="E32" s="11">
-        <v>350</v>
-      </c>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11">
-        <v>76</v>
+      <c r="A32" s="4">
+        <v>44</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E32" s="13">
+        <v>100</v>
+      </c>
+      <c r="F32" s="13">
+        <v>1</v>
+      </c>
+      <c r="G32" s="13">
+        <v>1</v>
+      </c>
+      <c r="H32" s="13">
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E33" s="13">
-        <v>250</v>
+        <v>20</v>
       </c>
       <c r="F33" s="13">
+        <v>4</v>
+      </c>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>46</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E34" s="13">
+        <v>140</v>
+      </c>
+      <c r="F34" s="13">
+        <v>1</v>
+      </c>
+      <c r="G34" s="13">
+        <v>1</v>
+      </c>
+      <c r="H34" s="13">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>47</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E35" s="13">
+        <v>200</v>
+      </c>
+      <c r="F35" s="13">
         <v>2</v>
       </c>
-      <c r="G33" s="13">
+      <c r="G35" s="13">
         <v>3</v>
       </c>
-      <c r="H33" s="13">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="3">
-        <v>37</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E34" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12">
+      <c r="H35" s="13">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>48</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E36" s="13">
+        <v>210</v>
+      </c>
+      <c r="F36" s="13">
+        <v>2</v>
+      </c>
+      <c r="G36" s="13">
+        <v>2</v>
+      </c>
+      <c r="H36" s="13">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>49</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E37" s="13">
+        <v>290</v>
+      </c>
+      <c r="F37" s="13">
         <v>3</v>
       </c>
-      <c r="H34" s="12">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="3">
-        <v>35</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="E35" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12">
-        <v>4</v>
-      </c>
-      <c r="H35" s="12">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
-        <v>39</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="F36" s="12"/>
-      <c r="G36" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="H36" s="12">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3">
-        <v>39.5</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E37" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="H37" s="12">
-        <v>110</v>
+      <c r="G37" s="13">
+        <v>1</v>
+      </c>
+      <c r="H37" s="13">
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -1816,7 +1816,7 @@
   </sheetData>
   <autoFilter ref="A1:H37">
     <sortState ref="A2:H37">
-      <sortCondition ref="H1:H37"/>
+      <sortCondition ref="A1:A37"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>